<commit_message>
Update 5modeling to use change in case rate as outcome. Use lme4 for modeling. Add in confidence interval estimates. Run models for each strategy as the only policy predictor then run with all in the same model.
</commit_message>
<xml_diff>
--- a/forest_list_statistics.xlsx
+++ b/forest_list_statistics.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,7 +366,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>positives</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ranks</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pos_ranked</t>
         </is>
       </c>
     </row>
@@ -379,6 +389,12 @@
       <c r="B2">
         <v>100</v>
       </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -387,6 +403,12 @@
         </is>
       </c>
       <c r="B3">
+        <v>94</v>
+      </c>
+      <c r="C3">
+        <v>87</v>
+      </c>
+      <c r="D3">
         <v>87</v>
       </c>
     </row>
@@ -397,6 +419,12 @@
         </is>
       </c>
       <c r="B4">
+        <v>66</v>
+      </c>
+      <c r="C4">
+        <v>54</v>
+      </c>
+      <c r="D4">
         <v>54</v>
       </c>
     </row>
@@ -407,6 +435,12 @@
         </is>
       </c>
       <c r="B5">
+        <v>57.99999999999999</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
         <v>44</v>
       </c>
     </row>
@@ -417,6 +451,12 @@
         </is>
       </c>
       <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+      <c r="D6">
         <v>42</v>
       </c>
     </row>
@@ -427,6 +467,12 @@
         </is>
       </c>
       <c r="B7">
+        <v>59</v>
+      </c>
+      <c r="C7">
+        <v>41</v>
+      </c>
+      <c r="D7">
         <v>41</v>
       </c>
     </row>
@@ -437,6 +483,12 @@
         </is>
       </c>
       <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8">
         <v>27</v>
       </c>
     </row>
@@ -447,26 +499,44 @@
         </is>
       </c>
       <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
         <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>locale</t>
+          <t>cntycaseschange</t>
         </is>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cntycaseschange</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11">
         <v>17</v>
       </c>
     </row>
@@ -477,6 +547,12 @@
         </is>
       </c>
       <c r="B12">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
         <v>12</v>
       </c>
     </row>
@@ -487,6 +563,12 @@
         </is>
       </c>
       <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
         <v>12</v>
       </c>
     </row>
@@ -497,6 +579,12 @@
         </is>
       </c>
       <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
@@ -507,6 +595,12 @@
         </is>
       </c>
       <c r="B15">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
         <v>6</v>
       </c>
     </row>
@@ -517,7 +611,13 @@
         </is>
       </c>
       <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
         <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +627,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -541,7 +641,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>positives</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ranks</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pos_ranked</t>
         </is>
       </c>
     </row>
@@ -554,6 +664,12 @@
       <c r="B2">
         <v>100</v>
       </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -562,6 +678,12 @@
         </is>
       </c>
       <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>99</v>
+      </c>
+      <c r="D3">
         <v>99</v>
       </c>
     </row>
@@ -572,67 +694,109 @@
         </is>
       </c>
       <c r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4">
         <v>51</v>
+      </c>
+      <c r="D4">
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cohortingorstaggering</t>
+          <t>etiquette</t>
         </is>
       </c>
       <c r="B5">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>etiquette</t>
+          <t>traceandquarantine</t>
         </is>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>traceandquarantine</t>
+          <t>masks</t>
         </is>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>ventilation</t>
         </is>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ventilation</t>
+          <t>cleaning</t>
         </is>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>7.000000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cleaning</t>
+          <t>cohortingorstaggering</t>
         </is>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -642,6 +806,12 @@
         </is>
       </c>
       <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 03identify_outliers.R. Updated model dataframes to exclude outliers.
</commit_message>
<xml_diff>
--- a/forest_list_statistics.xlsx
+++ b/forest_list_statistics.xlsx
@@ -383,7 +383,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B2">
@@ -399,59 +399,59 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>state</t>
         </is>
       </c>
       <c r="B3">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C3">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rplthemes</t>
+          <t>percenttwoormoreraces</t>
         </is>
       </c>
       <c r="B4">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C4">
-        <v>61</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="D4">
-        <v>61</v>
+        <v>57.99999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>derivedtotalenrolled</t>
+          <t>percentwhite</t>
         </is>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D5">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>percentblackorafricanamerican</t>
+          <t>rplthemes</t>
         </is>
       </c>
       <c r="B6">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>42</v>
@@ -463,65 +463,65 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>percentstudentsfreereducedlunch</t>
+          <t>percentblackorafricanamerican</t>
         </is>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>percentamericanindianoralaskanative</t>
+          <t>percentasian</t>
         </is>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D8">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>percenthispaniclatino</t>
+          <t>percentstudentsfreereducedlunch</t>
         </is>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>percenttwoormoreraces</t>
+          <t>percentamericanindianoralaskanative</t>
         </is>
       </c>
       <c r="B10">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -531,93 +531,93 @@
         </is>
       </c>
       <c r="B11">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>locale</t>
+          <t>percenthispaniclatino</t>
         </is>
       </c>
       <c r="B12">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>schoollevel</t>
+          <t>derivedtotalenrolled</t>
         </is>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>percentasian</t>
+          <t>percentnativehawaiianorotherpacificislander</t>
         </is>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>percentwhite</t>
+          <t>schoollevel</t>
         </is>
       </c>
       <c r="B15">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>percentnativehawaiianorotherpacificislander</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -627,10 +627,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -674,7 +674,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hvacsystems</t>
+          <t>cleaning</t>
         </is>
       </c>
       <c r="B2">
@@ -690,94 +690,94 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>contacttracing</t>
+          <t>physicaldistancing</t>
         </is>
       </c>
       <c r="B3">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C3">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D3">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>quarantine</t>
         </is>
       </c>
       <c r="B4">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D4">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>contacttracing</t>
         </is>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>screeningtestingforstudents</t>
+          <t>hvacsystems</t>
         </is>
       </c>
       <c r="B6">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C6">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cleaning</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>quarantine</t>
+          <t>masks</t>
         </is>
       </c>
       <c r="B8">
+        <v>22</v>
+      </c>
+      <c r="C8">
         <v>24</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
       </c>
       <c r="D8">
         <v>22</v>
@@ -786,17 +786,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>physicaldistancing</t>
+          <t>screeningtestingforstudents</t>
         </is>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <v>7.000000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -806,13 +806,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Add modeling results script and to report. Changed enrollment to 2020-21 school year figures. Fix issue #1, issue #2, and issue #3.
</commit_message>
<xml_diff>
--- a/forest_list_statistics.xlsx
+++ b/forest_list_statistics.xlsx
@@ -383,7 +383,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>state</t>
         </is>
       </c>
       <c r="B2">
@@ -399,17 +399,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
@@ -419,141 +419,141 @@
         </is>
       </c>
       <c r="B4">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C4">
-        <v>57.99999999999999</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>57.99999999999999</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>percentwhite</t>
+          <t>percentfreelunchqualified</t>
         </is>
       </c>
       <c r="B5">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>rplthemes</t>
+          <t>cntycaseschange</t>
         </is>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>percentblackorafricanamerican</t>
+          <t>percentwhite</t>
         </is>
       </c>
       <c r="B7">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>percentasian</t>
+          <t>percentamericanindianoralaskanative</t>
         </is>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="C8">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>percentstudentsfreereducedlunch</t>
+          <t>rplthemes</t>
         </is>
       </c>
       <c r="B9">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>percentamericanindianoralaskanative</t>
+          <t>percentblackorafricanamerican</t>
         </is>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cntycaseschange</t>
+          <t>percentnativehawaiianorotherpacificislander</t>
         </is>
       </c>
       <c r="B11">
-        <v>41</v>
+        <v>56.99999999999999</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>percenthispaniclatino</t>
+          <t>percentasian</t>
         </is>
       </c>
       <c r="B12">
         <v>34</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -563,29 +563,29 @@
         </is>
       </c>
       <c r="B13">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>percentnativehawaiianorotherpacificislander</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -595,29 +595,29 @@
         </is>
       </c>
       <c r="B15">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>locale</t>
+          <t>percenthispaniclatino</t>
         </is>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>7.000000000000001</v>
       </c>
     </row>
     <row r="17">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -674,129 +674,129 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cleaning</t>
+          <t>contacttracing</t>
         </is>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>physicaldistancing</t>
+          <t>hvacsystems</t>
         </is>
       </c>
       <c r="B3">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="C3">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D3">
-        <v>63</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>quarantine</t>
+          <t>cleaning</t>
         </is>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C4">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D4">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>contacttracing</t>
+          <t>screeningtestingforstudents</t>
         </is>
       </c>
       <c r="B5">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C5">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>56.99999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hvacsystems</t>
+          <t>quarantine</t>
         </is>
       </c>
       <c r="B6">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>masks</t>
         </is>
       </c>
       <c r="B7">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>physicaldistancing</t>
         </is>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>screeningtestingforstudents</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9">
-        <v>7.000000000000001</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -806,13 +806,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -822,13 +822,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finale modeling, including a cumulative strategy score. Reset outliers to be observations falling 3.5 SD outside mean of outcome variable.
</commit_message>
<xml_diff>
--- a/forest_list_statistics.xlsx
+++ b/forest_list_statistics.xlsx
@@ -383,7 +383,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B2">
@@ -399,17 +399,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>state</t>
         </is>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -419,77 +419,77 @@
         </is>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C4">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D4">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>percentfreelunchqualified</t>
+          <t>percentwhite</t>
         </is>
       </c>
       <c r="B5">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cntycaseschange</t>
+          <t>percentasian</t>
         </is>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="C6">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>percentwhite</t>
+          <t>percentfreelunchqualified</t>
         </is>
       </c>
       <c r="B7">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>percentamericanindianoralaskanative</t>
+          <t>percentblackorafricanamerican</t>
         </is>
       </c>
       <c r="B8">
-        <v>55.00000000000001</v>
+        <v>59</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -499,61 +499,61 @@
         </is>
       </c>
       <c r="B9">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>percentblackorafricanamerican</t>
+          <t>percenthispaniclatino</t>
         </is>
       </c>
       <c r="B10">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>percentnativehawaiianorotherpacificislander</t>
+          <t>percentamericanindianoralaskanative</t>
         </is>
       </c>
       <c r="B11">
-        <v>56.99999999999999</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>percentasian</t>
+          <t>schoollevel</t>
         </is>
       </c>
       <c r="B12">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -563,61 +563,61 @@
         </is>
       </c>
       <c r="B13">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="D13">
-        <v>13</v>
+        <v>7.000000000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>locale</t>
+          <t>cntycaseschange</t>
         </is>
       </c>
       <c r="B14">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>schoollevel</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B15">
         <v>30</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>percenthispaniclatino</t>
+          <t>percentnativehawaiianorotherpacificislander</t>
         </is>
       </c>
       <c r="B16">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C16">
-        <v>7.000000000000001</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>7.000000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -678,13 +678,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
@@ -694,13 +694,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D3">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
@@ -710,13 +710,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C4">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -726,93 +726,93 @@
         </is>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D5">
-        <v>56.99999999999999</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>quarantine</t>
+          <t>masks</t>
         </is>
       </c>
       <c r="B6">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>physicaldistancing</t>
         </is>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>physicaldistancing</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>hepafilters</t>
         </is>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hepafilters</t>
+          <t>quarantine</t>
         </is>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -822,13 +822,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>